<commit_message>
Fixes to currency conversions
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\South Korea\Models\eps-southkorea\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99DAB2E-C1FB-4D17-8424-6CB545CE53D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB5FE3D-9B81-4B3E-A24B-23B2DFEABBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11930" yWindow="0" windowWidth="13460" windowHeight="13700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +148,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,8 +184,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -190,10 +199,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,32 +542,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,80 +575,80 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.89805481563188172</v>
       </c>
@@ -646,55 +656,58 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="9" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B36">
         <v>1164.79</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="9" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C36" r:id="rId1" xr:uid="{1D3CC4E1-E398-4D6F-B67D-99A925F86565}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -709,23 +722,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3">
-        <f>10^9*About!$A$26*About!$B$36</f>
-        <v>1046045268699.8595</v>
+        <f>1/(10^9*About!$A$26*About!$B$36)</f>
+        <v>9.5598157166076601E-13</v>
       </c>
     </row>
   </sheetData>
@@ -741,26 +754,26 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8">
-        <f>10^6*About!$A$26*About!$B$36</f>
-        <v>1046045268.6998595</v>
+      <c r="B2" s="3">
+        <f>1/(10^6*About!$A$26*About!$B$36)</f>
+        <v>9.5598157166076609E-10</v>
       </c>
     </row>
   </sheetData>
@@ -775,27 +788,27 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7">
-        <f>1*About!A26*About!$B$36</f>
-        <v>1046.0452686998594</v>
+        <f>1/(About!A26*About!$B$36)</f>
+        <v>9.559815716607661E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>